<commit_message>
insert db by excel
</commit_message>
<xml_diff>
--- a/DoAnHTTT/src/main/webapp/File/1.xlsx
+++ b/DoAnHTTT/src/main/webapp/File/1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID_Student</t>
   </si>
@@ -51,40 +51,16 @@
     <t>DH18DTA</t>
   </si>
   <si>
-    <t>Đàm Văn Anh A</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh B</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh C</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh D</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh E</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh F</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh G</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh H</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh I</t>
-  </si>
-  <si>
-    <t>Đàm Văn Anh J</t>
+    <t>"18130009"</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,8 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,11 +415,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>18130005</v>
+      <c r="A2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -459,214 +437,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>18130005</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>136</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>18130005</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>136</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>18130005</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>136</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>18130005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>136</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>18130005</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>136</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>18130005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>136</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>18130005</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>136</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>18130005</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>136</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>18130005</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <v>136</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>